<commit_message>
more updates to Table 1 (added two outcomes we created for CTN-0094)
</commit_message>
<xml_diff>
--- a/inst/suppl_docs/definitions_20220405.xlsx
+++ b/inst/suppl_docs/definitions_20220405.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielodom/Documents/GitHub/CTN-0094/CTNote/inst/suppl_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C5C5C7-0433-D541-A05F-C51370C30433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E18D71FE-14F5-D043-9887-6BF4983C5122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{5E30E9EF-9AAA-CD48-B338-97B5233CAF9E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="224">
   <si>
     <t>Primary Endpoint</t>
   </si>
@@ -966,12 +966,36 @@
   <si>
     <t>attaining at least 3 weeks of consecutive negative UOS</t>
   </si>
+  <si>
+    <t>Time to relapse</t>
+  </si>
+  <si>
+    <t>Time to study dropout</t>
+  </si>
+  <si>
+    <t>CTN-0094</t>
+  </si>
+  <si>
+    <t>Weeks to relapse (4 consecutive weeks of positive UOS)</t>
+  </si>
+  <si>
+    <t>Weeks to study dropout (4 consecutive weeks of missing UOS)</t>
+  </si>
+  <si>
+    <t>relapse_time, relapse_event</t>
+  </si>
+  <si>
+    <t>dropout_time, dropout_event</t>
+  </si>
+  <si>
+    <t>eissenberg1997_abs</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1053,6 +1077,13 @@
       <name val="Cambria Math"/>
       <family val="1"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1068,7 +1099,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1167,11 +1198,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1218,6 +1271,16 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1532,10 +1595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A1123D4-B217-1541-959A-BB4DAF6F68A4}">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1907,10 +1970,10 @@
       <c r="C13" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="18" t="s">
         <v>213</v>
       </c>
       <c r="F13" s="9" t="s">
@@ -1922,269 +1985,265 @@
       <c r="H13" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I13" s="14" t="s">
+      <c r="I13" s="19" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>36</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>37</v>
+        <v>216</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="23" t="s">
+        <v>218</v>
+      </c>
+      <c r="E14" s="15"/>
+      <c r="F14" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>218</v>
+      </c>
+      <c r="E15" s="21"/>
+      <c r="F15" s="22" t="s">
+        <v>220</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="21" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E16" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F16" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="I16" s="14" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.2">
-      <c r="A16" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="14" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>41</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>36</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I19" s="14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E20" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I18" s="14" t="s">
+      <c r="I20" s="14" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="61" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+    <row r="21" spans="1:9" ht="61" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B21" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C21" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D21" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E21" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F21" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G21" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="H21" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I19" s="14" t="s">
+      <c r="I21" s="19" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.2">
-      <c r="A20" s="12" t="s">
+    <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B22" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C22" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D22" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E22" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F22" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H22" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I20" s="14" t="s">
+      <c r="I22" s="14" t="s">
         <v>128</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A21" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I21" s="14" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.2">
-      <c r="A22" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>206</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I22" s="14" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -2195,28 +2254,28 @@
         <v>51</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>131</v>
+        <v>55</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>50</v>
       </c>
@@ -2227,25 +2286,25 @@
         <v>114</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>162</v>
+        <v>10</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>50</v>
       </c>
@@ -2256,23 +2315,25 @@
         <v>114</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>168</v>
+        <v>185</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>164</v>
+        <v>131</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="I25" s="14"/>
-    </row>
-    <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="I25" s="14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
         <v>50</v>
       </c>
@@ -2283,25 +2344,25 @@
         <v>114</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>46</v>
+        <v>162</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>50</v>
       </c>
@@ -2309,25 +2370,25 @@
         <v>51</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>212</v>
+        <v>168</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>67</v>
+        <v>164</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>46</v>
+        <v>162</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>135</v>
+        <v>223</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="45" x14ac:dyDescent="0.2">
@@ -2341,22 +2402,22 @@
         <v>114</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="I28" s="14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -2367,25 +2428,25 @@
         <v>51</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>16</v>
+        <v>116</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>26</v>
+        <v>212</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="I29" s="14" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.2">
@@ -2398,81 +2459,81 @@
       <c r="C30" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>73</v>
+      <c r="D30" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>205</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>10</v>
+        <v>197</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="I30" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>110</v>
+      <c r="B31" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="I31" s="14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>110</v>
+      <c r="B32" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>175</v>
+        <v>73</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>174</v>
+        <v>205</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -2483,57 +2544,57 @@
         <v>75</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>183</v>
+        <v>208</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I33" s="14" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>50</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>114</v>
+      <c r="C34" s="16" t="s">
+        <v>110</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>83</v>
+        <v>175</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>188</v>
+        <v>79</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I34" s="14" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
         <v>50</v>
       </c>
@@ -2544,25 +2605,25 @@
         <v>114</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>189</v>
+        <v>81</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I35" s="14" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
         <v>50</v>
       </c>
@@ -2573,22 +2634,22 @@
         <v>114</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>169</v>
+        <v>187</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>85</v>
+        <v>188</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I36" s="14" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="60" x14ac:dyDescent="0.2">
@@ -2599,25 +2660,25 @@
         <v>75</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E37" s="17" t="s">
-        <v>209</v>
+        <v>187</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>87</v>
+        <v>189</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I37" s="14" t="s">
-        <v>165</v>
+        <v>190</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -2631,13 +2692,13 @@
         <v>114</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>11</v>
@@ -2646,7 +2707,7 @@
         <v>15</v>
       </c>
       <c r="I38" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="60" x14ac:dyDescent="0.2">
@@ -2657,28 +2718,28 @@
         <v>75</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>114</v>
+        <v>139</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="E39" s="17" t="s">
-        <v>186</v>
+        <v>209</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>91</v>
+        <v>11</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I39" s="14" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
         <v>50</v>
       </c>
@@ -2689,25 +2750,25 @@
         <v>114</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>207</v>
+        <v>171</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I40" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
         <v>50</v>
       </c>
@@ -2718,22 +2779,22 @@
         <v>114</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>94</v>
+        <v>30</v>
       </c>
       <c r="E41" s="17" t="s">
-        <v>167</v>
+        <v>186</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I41" s="14" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.2">
@@ -2747,22 +2808,22 @@
         <v>114</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E42" s="17" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>163</v>
+        <v>9</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="I42" s="14" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -2776,25 +2837,25 @@
         <v>114</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>7</v>
+        <v>94</v>
       </c>
       <c r="E43" s="17" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>150</v>
+        <v>95</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I43" s="14" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="s">
         <v>50</v>
       </c>
@@ -2802,28 +2863,28 @@
         <v>75</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>7</v>
+        <v>96</v>
       </c>
       <c r="E44" s="17" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>151</v>
+        <v>97</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>163</v>
       </c>
       <c r="I44" s="14" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="75" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A45" s="12" t="s">
         <v>50</v>
       </c>
@@ -2834,25 +2895,25 @@
         <v>114</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>98</v>
+        <v>7</v>
       </c>
       <c r="E45" s="17" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>193</v>
+        <v>150</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I45" s="14" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A46" s="12" t="s">
         <v>50</v>
       </c>
@@ -2860,28 +2921,28 @@
         <v>75</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>98</v>
+        <v>7</v>
       </c>
       <c r="E46" s="17" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>195</v>
+        <v>151</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I46" s="14" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="75" x14ac:dyDescent="0.2">
       <c r="A47" s="12" t="s">
         <v>50</v>
       </c>
@@ -2892,25 +2953,25 @@
         <v>114</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E47" s="17" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>100</v>
+        <v>193</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H47" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I47" s="14" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A48" s="12" t="s">
         <v>50</v>
       </c>
@@ -2921,25 +2982,25 @@
         <v>114</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="E48" s="17" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>101</v>
+        <v>195</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="I48" s="14" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A49" s="12" t="s">
         <v>50</v>
       </c>
@@ -2950,25 +3011,25 @@
         <v>114</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E49" s="17" t="s">
-        <v>170</v>
+        <v>198</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="I49" s="14" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A50" s="12" t="s">
         <v>50</v>
       </c>
@@ -2979,25 +3040,25 @@
         <v>114</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>103</v>
+        <v>24</v>
       </c>
       <c r="E50" s="17" t="s">
-        <v>172</v>
+        <v>200</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>162</v>
+        <v>26</v>
       </c>
       <c r="I50" s="14" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A51" s="12" t="s">
         <v>50</v>
       </c>
@@ -3008,21 +3069,79 @@
         <v>114</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>173</v>
+        <v>102</v>
+      </c>
+      <c r="E51" s="17" t="s">
+        <v>170</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H51" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I51" s="14" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+      <c r="A52" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E52" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="I52" s="14" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+      <c r="A53" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H53" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I51" s="15" t="s">
+      <c r="I53" s="15" t="s">
         <v>158</v>
       </c>
     </row>

</xml_diff>

<commit_message>
I was missing some of the correct coded names
</commit_message>
<xml_diff>
--- a/inst/suppl_docs/definitions_20220405.xlsx
+++ b/inst/suppl_docs/definitions_20220405.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielodom/Documents/GitHub/CTN-0094/CTNote/inst/suppl_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E18D71FE-14F5-D043-9887-6BF4983C5122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE9C3F8-F1D7-4A4F-A7F0-D5AE142E655E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{5E30E9EF-9AAA-CD48-B338-97B5233CAF9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="228">
   <si>
     <t>Primary Endpoint</t>
   </si>
@@ -665,12 +666,6 @@
     <t>lee2018_rel_time, lee2018_rel_event</t>
   </si>
   <si>
-    <t>krupitsky2004_rel</t>
-  </si>
-  <si>
-    <t>johnson1992_rel</t>
-  </si>
-  <si>
     <t>sokya2008_abs, sokya2008_use</t>
   </si>
   <si>
@@ -707,63 +702,15 @@
     <t>NA</t>
   </si>
   <si>
-    <t>strang2010</t>
-  </si>
-  <si>
-    <t>ling2010</t>
-  </si>
-  <si>
-    <t>fiellin2006</t>
-  </si>
-  <si>
-    <t>haight2019</t>
-  </si>
-  <si>
     <t>lofwall2018_abs</t>
   </si>
   <si>
-    <t>lofwall2018</t>
-  </si>
-  <si>
-    <t>strang2019</t>
-  </si>
-  <si>
-    <t>comer2006</t>
-  </si>
-  <si>
-    <t>kosten1993B</t>
-  </si>
-  <si>
-    <t>wolstein2009</t>
-  </si>
-  <si>
     <t>Mean percentage negative UOS</t>
   </si>
   <si>
     <t>no. of negative UOS (“treatment effectiveness score”)</t>
   </si>
   <si>
-    <t>ling1998A</t>
-  </si>
-  <si>
-    <t>ling1998C</t>
-  </si>
-  <si>
-    <t>preston2000</t>
-  </si>
-  <si>
-    <t>schottenfeld2005</t>
-  </si>
-  <si>
-    <t>fudala2003</t>
-  </si>
-  <si>
-    <t>jaffe1972</t>
-  </si>
-  <si>
-    <t>johnson1992</t>
-  </si>
-  <si>
     <t>kosten1993_abs</t>
   </si>
   <si>
@@ -780,9 +727,6 @@
   </si>
   <si>
     <t>subject retained in study at least 17 weeks AND subject showed 4 consecutive negative UDS between weeks 1-17</t>
-  </si>
-  <si>
-    <t>mattick2003A</t>
   </si>
   <si>
     <t>DOI</t>
@@ -877,9 +821,6 @@
     </r>
   </si>
   <si>
-    <t>mattick2003B</t>
-  </si>
-  <si>
     <t>https://doi.org/10.1111/add.13259</t>
   </si>
   <si>
@@ -889,13 +830,7 @@
     <t>PCC: Percentage ratio of negative UOS and the total number of UOS carried out for each patient during the period of treatment</t>
   </si>
   <si>
-    <t>pani2000A</t>
-  </si>
-  <si>
     <t>TEC: Percentage ratio between the number of negative UOS and the number of UOS as per protocol</t>
-  </si>
-  <si>
-    <t>pani2000B</t>
   </si>
   <si>
     <t>https://doi.org/10.1016/S0376-8716(00)00163-0</t>
@@ -989,6 +924,84 @@
   </si>
   <si>
     <t>eissenberg1997_abs</t>
+  </si>
+  <si>
+    <t>comer2006_red</t>
+  </si>
+  <si>
+    <t>fiellin2006_red</t>
+  </si>
+  <si>
+    <t>fudala2003_red</t>
+  </si>
+  <si>
+    <t>haight2019_red</t>
+  </si>
+  <si>
+    <t>jaffe1972_red</t>
+  </si>
+  <si>
+    <t>johnson1992_red</t>
+  </si>
+  <si>
+    <t>johnson1992_rel, johnson1992_abs</t>
+  </si>
+  <si>
+    <t>kosten1993B_red</t>
+  </si>
+  <si>
+    <t>krupitsky2004_rel, krupitsky2004_abs</t>
+  </si>
+  <si>
+    <t>ling1998A_red</t>
+  </si>
+  <si>
+    <t>ling1998C_red</t>
+  </si>
+  <si>
+    <t>ling2010_red</t>
+  </si>
+  <si>
+    <t>lofwall2018_red</t>
+  </si>
+  <si>
+    <t>mattick2003A_red</t>
+  </si>
+  <si>
+    <t>mattick2003B_red</t>
+  </si>
+  <si>
+    <t>pani2000A_red</t>
+  </si>
+  <si>
+    <t>pani2000B_red</t>
+  </si>
+  <si>
+    <t>preston2000_red</t>
+  </si>
+  <si>
+    <t>schottenfeld2005_red</t>
+  </si>
+  <si>
+    <t>Strain, Bigelow, Liebson, &amp; Stitzer, 1999</t>
+  </si>
+  <si>
+    <t>strain1999A_abs, strain19969_use</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1001/jama.281.11.1000</t>
+  </si>
+  <si>
+    <t>strang2010_red</t>
+  </si>
+  <si>
+    <t>strang2019_red</t>
+  </si>
+  <si>
+    <t>tanum2017_red</t>
+  </si>
+  <si>
+    <t>wolstein2009_red</t>
   </si>
 </sst>
 </file>
@@ -1099,7 +1112,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1220,11 +1233,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1279,6 +1301,14 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1595,11 +1625,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A1123D4-B217-1541-959A-BB4DAF6F68A4}">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1626,7 +1654,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>2</v>
@@ -1654,8 +1682,8 @@
       <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="17" t="s">
-        <v>184</v>
+      <c r="E2" s="25" t="s">
+        <v>165</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>8</v>
@@ -1667,7 +1695,7 @@
         <v>10</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -1681,13 +1709,13 @@
         <v>110</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>215</v>
+        <v>193</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>11</v>
@@ -1696,7 +1724,7 @@
         <v>10</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.2">
@@ -1713,7 +1741,7 @@
         <v>13</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>199</v>
+        <v>177</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>14</v>
@@ -1742,7 +1770,7 @@
         <v>16</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>202</v>
+        <v>180</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>17</v>
@@ -1771,7 +1799,7 @@
         <v>18</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>19</v>
@@ -1800,7 +1828,7 @@
         <v>22</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>199</v>
+        <v>177</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>23</v>
@@ -1829,7 +1857,7 @@
         <v>24</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>200</v>
+        <v>178</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>25</v>
@@ -1858,7 +1886,7 @@
         <v>28</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>29</v>
@@ -1887,7 +1915,7 @@
         <v>30</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>120</v>
@@ -1899,7 +1927,7 @@
         <v>15</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -1916,7 +1944,7 @@
         <v>84</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>33</v>
@@ -1945,19 +1973,19 @@
         <v>28</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="61" thickBot="1" x14ac:dyDescent="0.25">
@@ -1971,10 +1999,10 @@
         <v>110</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>214</v>
+        <v>192</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>213</v>
+        <v>191</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>35</v>
@@ -1994,17 +2022,17 @@
         <v>36</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>216</v>
+        <v>194</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>111</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>218</v>
+        <v>196</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="22" t="s">
-        <v>219</v>
+        <v>197</v>
       </c>
       <c r="G14" s="22" t="s">
         <v>11</v>
@@ -2013,7 +2041,7 @@
         <v>15</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>221</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.2">
@@ -2021,17 +2049,17 @@
         <v>36</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>217</v>
+        <v>195</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>111</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>218</v>
+        <v>196</v>
       </c>
       <c r="E15" s="21"/>
       <c r="F15" s="22" t="s">
-        <v>220</v>
+        <v>198</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>11</v>
@@ -2040,7 +2068,7 @@
         <v>26</v>
       </c>
       <c r="I15" s="21" t="s">
-        <v>222</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -2057,7 +2085,7 @@
         <v>22</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>199</v>
+        <v>177</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>38</v>
@@ -2072,7 +2100,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>36</v>
       </c>
@@ -2086,7 +2114,7 @@
         <v>39</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>40</v>
@@ -2101,7 +2129,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>36</v>
       </c>
@@ -2115,7 +2143,7 @@
         <v>42</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>43</v>
@@ -2130,7 +2158,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>36</v>
       </c>
@@ -2143,8 +2171,8 @@
       <c r="D19" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E19" s="17" t="s">
-        <v>177</v>
+      <c r="E19" s="25" t="s">
+        <v>158</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>45</v>
@@ -2156,10 +2184,10 @@
         <v>46</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>36</v>
       </c>
@@ -2170,10 +2198,10 @@
         <v>110</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>178</v>
+        <v>157</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>159</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>45</v>
@@ -2185,10 +2213,10 @@
         <v>46</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="61" thickBot="1" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="61" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>36</v>
       </c>
@@ -2202,7 +2230,7 @@
         <v>47</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>48</v>
@@ -2214,10 +2242,10 @@
         <v>15</v>
       </c>
       <c r="I21" s="19" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>50</v>
       </c>
@@ -2231,7 +2259,7 @@
         <v>52</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>203</v>
+        <v>181</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>53</v>
@@ -2243,10 +2271,10 @@
         <v>10</v>
       </c>
       <c r="I22" s="14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>50</v>
       </c>
@@ -2260,7 +2288,7 @@
         <v>54</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>201</v>
+        <v>179</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>55</v>
@@ -2272,10 +2300,10 @@
         <v>10</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>50</v>
       </c>
@@ -2289,7 +2317,7 @@
         <v>57</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>206</v>
+        <v>184</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>58</v>
@@ -2301,10 +2329,10 @@
         <v>10</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>50</v>
       </c>
@@ -2318,10 +2346,10 @@
         <v>59</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>11</v>
@@ -2330,10 +2358,10 @@
         <v>15</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
         <v>50</v>
       </c>
@@ -2347,7 +2375,7 @@
         <v>60</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>211</v>
+        <v>189</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>61</v>
@@ -2356,13 +2384,13 @@
         <v>62</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>50</v>
       </c>
@@ -2376,22 +2404,22 @@
         <v>63</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>50</v>
       </c>
@@ -2405,7 +2433,7 @@
         <v>64</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>65</v>
@@ -2417,10 +2445,10 @@
         <v>46</v>
       </c>
       <c r="I28" s="14" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>50</v>
       </c>
@@ -2433,8 +2461,8 @@
       <c r="D29" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E29" s="17" t="s">
-        <v>212</v>
+      <c r="E29" s="25" t="s">
+        <v>190</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>67</v>
@@ -2446,11 +2474,11 @@
         <v>46</v>
       </c>
       <c r="I29" s="14" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.2">
-      <c r="A30" s="12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+      <c r="A30" s="26" t="s">
         <v>50</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -2460,25 +2488,27 @@
         <v>114</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>197</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>69</v>
+        <v>221</v>
+      </c>
+      <c r="E30" t="s">
+        <v>223</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I30" s="14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+      <c r="J30" s="27"/>
+      <c r="K30" s="24"/>
+    </row>
+    <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>50</v>
       </c>
@@ -2488,26 +2518,26 @@
       <c r="C31" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>16</v>
+      <c r="D31" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>26</v>
+        <v>175</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="I31" s="14" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
         <v>50</v>
       </c>
@@ -2518,51 +2548,51 @@
         <v>114</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>205</v>
+        <v>180</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>110</v>
+      <c r="B33" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>208</v>
+        <v>183</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I33" s="14" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -2572,26 +2602,26 @@
       <c r="B34" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="2" t="s">
         <v>110</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>175</v>
+        <v>76</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>174</v>
+        <v>186</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I34" s="14" t="s">
-        <v>148</v>
+        <v>224</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -2601,29 +2631,29 @@
       <c r="B35" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>114</v>
+      <c r="C35" s="16" t="s">
+        <v>110</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E35" s="17" t="s">
-        <v>183</v>
+        <v>156</v>
+      </c>
+      <c r="E35" s="25" t="s">
+        <v>155</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>82</v>
+        <v>11</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I35" s="14" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
         <v>50</v>
       </c>
@@ -2634,22 +2664,22 @@
         <v>114</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>187</v>
+        <v>164</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>188</v>
+        <v>81</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I36" s="14" t="s">
-        <v>165</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="60" x14ac:dyDescent="0.2">
@@ -2666,10 +2696,10 @@
         <v>83</v>
       </c>
       <c r="E37" s="17" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>41</v>
@@ -2678,10 +2708,10 @@
         <v>10</v>
       </c>
       <c r="I37" s="14" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
         <v>50</v>
       </c>
@@ -2692,25 +2722,25 @@
         <v>114</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>85</v>
+        <v>170</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I38" s="14" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
         <v>50</v>
       </c>
@@ -2718,16 +2748,16 @@
         <v>75</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E39" s="17" t="s">
-        <v>209</v>
+        <v>150</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>11</v>
@@ -2736,10 +2766,10 @@
         <v>15</v>
       </c>
       <c r="I39" s="14" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
         <v>50</v>
       </c>
@@ -2747,16 +2777,16 @@
         <v>75</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>11</v>
@@ -2764,11 +2794,11 @@
       <c r="H40" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I40" s="14" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+      <c r="I40" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
         <v>50</v>
       </c>
@@ -2779,25 +2809,25 @@
         <v>114</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="E41" s="17" t="s">
-        <v>186</v>
+        <v>152</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>91</v>
+        <v>11</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I41" s="14" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A42" s="12" t="s">
         <v>50</v>
       </c>
@@ -2808,25 +2838,25 @@
         <v>114</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>92</v>
+        <v>30</v>
       </c>
       <c r="E42" s="17" t="s">
-        <v>207</v>
+        <v>167</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I42" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
         <v>50</v>
       </c>
@@ -2837,25 +2867,25 @@
         <v>114</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E43" s="17" t="s">
-        <v>167</v>
+        <v>185</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I43" s="14" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="s">
         <v>50</v>
       </c>
@@ -2866,25 +2896,25 @@
         <v>114</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E44" s="17" t="s">
-        <v>210</v>
+        <v>148</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H44" s="3" t="s">
-        <v>163</v>
+        <v>20</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="I44" s="14" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A45" s="12" t="s">
         <v>50</v>
       </c>
@@ -2895,22 +2925,22 @@
         <v>114</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>7</v>
+        <v>96</v>
       </c>
       <c r="E45" s="17" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>150</v>
+        <v>97</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>145</v>
       </c>
       <c r="I45" s="14" t="s">
-        <v>152</v>
+        <v>227</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -2921,16 +2951,16 @@
         <v>75</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E46" s="17" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>9</v>
@@ -2939,10 +2969,10 @@
         <v>10</v>
       </c>
       <c r="I46" s="14" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="75" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A47" s="12" t="s">
         <v>50</v>
       </c>
@@ -2950,28 +2980,28 @@
         <v>75</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>98</v>
+        <v>7</v>
       </c>
       <c r="E47" s="17" t="s">
-        <v>192</v>
+        <v>165</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>193</v>
+        <v>140</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I47" s="14" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="75" x14ac:dyDescent="0.2">
       <c r="A48" s="12" t="s">
         <v>50</v>
       </c>
@@ -2985,10 +3015,10 @@
         <v>98</v>
       </c>
       <c r="E48" s="17" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>11</v>
@@ -2997,7 +3027,7 @@
         <v>15</v>
       </c>
       <c r="I48" s="14" t="s">
-        <v>196</v>
+        <v>217</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="60" x14ac:dyDescent="0.2">
@@ -3011,25 +3041,25 @@
         <v>114</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E49" s="17" t="s">
-        <v>198</v>
+        <v>172</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>100</v>
+        <v>174</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H49" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I49" s="14" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A50" s="12" t="s">
         <v>50</v>
       </c>
@@ -3040,22 +3070,22 @@
         <v>114</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="E50" s="17" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="I50" s="14" t="s">
-        <v>155</v>
+        <v>219</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.2">
@@ -3069,13 +3099,13 @@
         <v>114</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="E51" s="17" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>9</v>
@@ -3084,10 +3114,10 @@
         <v>26</v>
       </c>
       <c r="I51" s="14" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A52" s="12" t="s">
         <v>50</v>
       </c>
@@ -3098,25 +3128,25 @@
         <v>114</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E52" s="17" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>162</v>
+        <v>26</v>
       </c>
       <c r="I52" s="14" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A53" s="12" t="s">
         <v>50</v>
       </c>
@@ -3127,22 +3157,51 @@
         <v>114</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>173</v>
+        <v>103</v>
+      </c>
+      <c r="E53" s="17" t="s">
+        <v>153</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H53" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I53" s="14" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+      <c r="A54" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H54" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I53" s="15" t="s">
-        <v>158</v>
+      <c r="I54" s="15" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed "missing as" based on comment from Laura
</commit_message>
<xml_diff>
--- a/inst/suppl_docs/definitions_20220405.xlsx
+++ b/inst/suppl_docs/definitions_20220405.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielodom/Documents/GitHub/CTN-0094/CTNote/inst/suppl_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE9C3F8-F1D7-4A4F-A7F0-D5AE142E655E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01826DD1-87EC-3445-81B3-9E26F0ABD995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{5E30E9EF-9AAA-CD48-B338-97B5233CAF9E}"/>
   </bookViews>
@@ -1627,7 +1627,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A1123D4-B217-1541-959A-BB4DAF6F68A4}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2181,7 +2183,7 @@
         <v>41</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="I19" s="14" t="s">
         <v>210</v>
@@ -2210,7 +2212,7 @@
         <v>41</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="I20" s="14" t="s">
         <v>210</v>

</xml_diff>

<commit_message>
more minor edits to Table 1
</commit_message>
<xml_diff>
--- a/inst/suppl_docs/definitions_20220405.xlsx
+++ b/inst/suppl_docs/definitions_20220405.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielodom/Documents/GitHub/CTN-0094/CTNote/inst/suppl_docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\godom\GitHub\CTN-0094\CTNote\inst\suppl_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01826DD1-87EC-3445-81B3-9E26F0ABD995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7430747C-D465-4892-AA83-E52BBD93DD9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{5E30E9EF-9AAA-CD48-B338-97B5233CAF9E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5E30E9EF-9AAA-CD48-B338-97B5233CAF9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -61,9 +61,6 @@
     <t>Ling et al., 1998</t>
   </si>
   <si>
-    <t>% of participants who maintained 13 consecutive negative UOS</t>
-  </si>
-  <si>
     <t>3x/week</t>
   </si>
   <si>
@@ -1002,6 +999,9 @@
   </si>
   <si>
     <t>wolstein2009_red</t>
+  </si>
+  <si>
+    <t>% of participants who maintained 13 consecutive negative UOS (1 month)</t>
   </si>
 </sst>
 </file>
@@ -1627,36 +1627,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A1123D4-B217-1541-959A-BB4DAF6F68A4}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" customWidth="1"/>
-    <col min="4" max="5" width="16.6640625" customWidth="1"/>
-    <col min="6" max="6" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.83203125" customWidth="1"/>
+    <col min="1" max="1" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.375" customWidth="1"/>
+    <col min="4" max="5" width="16.625" customWidth="1"/>
+    <col min="6" max="6" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.875" customWidth="1"/>
     <col min="9" max="9" width="52" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="46" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>2</v>
@@ -1668,10 +1668,10 @@
         <v>4</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>5</v>
       </c>
@@ -1679,28 +1679,28 @@
         <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="I2" s="14" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>5</v>
       </c>
@@ -1708,1502 +1708,1502 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="47" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="H6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="E7" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="I8" s="14" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="116.25" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="17" t="s">
-        <v>160</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="G9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="204" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="H10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="17" t="s">
+      <c r="G12" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="61" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="F13" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="G13" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="19" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.2">
-      <c r="A14" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>111</v>
-      </c>
       <c r="D14" s="23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G14" s="22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H14" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D15" s="23" t="s">
         <v>195</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>196</v>
       </c>
       <c r="E15" s="21"/>
       <c r="F15" s="22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I15" s="21" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="130.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="57" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="14" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="14" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="19" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I22" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I25" s="14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I26" s="14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="57" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I27" s="14" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A16" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G16" s="4" t="s">
+    <row r="28" spans="1:11" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I28" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I29" s="14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E30" t="s">
+        <v>222</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="14" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" s="14" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="60" x14ac:dyDescent="0.2">
-      <c r="A18" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I18" s="14" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.2">
-      <c r="A19" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E19" s="25" t="s">
-        <v>158</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I19" s="14" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.2">
-      <c r="A20" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E20" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" s="14" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="61" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="H21" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I21" s="19" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.2">
-      <c r="A22" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I22" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.2">
-      <c r="A23" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E23" s="17" t="s">
-        <v>179</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I23" s="14" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="45" x14ac:dyDescent="0.2">
-      <c r="A24" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>184</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I24" s="14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.2">
-      <c r="A25" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I25" s="14" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.2">
-      <c r="A26" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>189</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="I26" s="14" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="60" x14ac:dyDescent="0.2">
-      <c r="A27" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="I27" s="14" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="45" x14ac:dyDescent="0.2">
-      <c r="A28" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I28" s="14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="30" x14ac:dyDescent="0.2">
-      <c r="A29" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E29" s="25" t="s">
-        <v>190</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I29" s="14" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.2">
-      <c r="A30" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D30" s="1" t="s">
+      <c r="I30" s="14" t="s">
         <v>221</v>
-      </c>
-      <c r="E30" t="s">
-        <v>223</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I30" s="14" t="s">
-        <v>222</v>
       </c>
       <c r="J30" s="27"/>
       <c r="K30" s="24"/>
     </row>
-    <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="C31" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E31" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F31" s="1" t="s">
+      <c r="G31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I31" s="14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I31" s="14" t="s">
+      <c r="G32" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I32" s="14" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="30" x14ac:dyDescent="0.2">
-      <c r="A32" s="12" t="s">
+    <row r="33" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E32" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I32" s="14" t="s">
+      <c r="C33" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I33" s="14" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="45" x14ac:dyDescent="0.2">
-      <c r="A33" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>183</v>
-      </c>
-      <c r="F33" s="2" t="s">
+    <row r="34" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="C34" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I34" s="14" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E35" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H35" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="I35" s="14" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I36" s="14" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="57" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I37" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="130.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I38" s="14" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I33" s="14" t="s">
+      <c r="H39" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I39" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="57" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A34" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E34" s="17" t="s">
+      <c r="D40" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E40" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="F34" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I34" s="14" t="s">
+      <c r="F40" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I40" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I41" s="14" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="204" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I42" s="14" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="116.25" x14ac:dyDescent="0.25">
+      <c r="A43" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I43" s="14" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A35" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E35" s="25" t="s">
-        <v>155</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H35" s="2" t="s">
+    <row r="44" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I44" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E45" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G45" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I35" s="14" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A36" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E36" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I36" s="14" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="60" x14ac:dyDescent="0.2">
-      <c r="A37" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E37" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I37" s="14" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="60" x14ac:dyDescent="0.2">
-      <c r="A38" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E38" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I38" s="14" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A39" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E39" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I39" s="14" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="60" x14ac:dyDescent="0.2">
-      <c r="A40" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E40" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I40" t="s">
+      <c r="H45" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="I45" s="14" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A41" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E41" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I41" s="14" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="60" x14ac:dyDescent="0.2">
-      <c r="A42" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E42" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I42" s="14" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.2">
-      <c r="A43" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E43" s="17" t="s">
-        <v>185</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I43" s="14" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A44" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E44" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I44" s="14" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="45" x14ac:dyDescent="0.2">
-      <c r="A45" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E45" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="I45" s="14" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E46" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G46" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H46" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H46" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="I46" s="14" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E47" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G47" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H47" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H47" s="2" t="s">
+      <c r="I47" s="14" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="A48" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E48" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G48" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I47" s="14" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="75" x14ac:dyDescent="0.2">
-      <c r="A48" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D48" s="2" t="s">
+      <c r="H48" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I48" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="57" x14ac:dyDescent="0.25">
+      <c r="A49" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E49" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I49" s="14" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="57" x14ac:dyDescent="0.25">
+      <c r="A50" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E48" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I48" s="14" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="60" x14ac:dyDescent="0.2">
-      <c r="A49" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E49" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I49" s="14" t="s">
+      <c r="E50" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I50" s="14" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="60" x14ac:dyDescent="0.2">
-      <c r="A50" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E50" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="F50" s="2" t="s">
+    <row r="51" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E51" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="F51" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="G50" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I50" s="14" t="s">
+      <c r="G51" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I51" s="14" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A51" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E51" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="F51" s="2" t="s">
+    <row r="52" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A52" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G51" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I51" s="14" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A52" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D52" s="2" t="s">
+      <c r="E52" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I52" s="14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="57" x14ac:dyDescent="0.25">
+      <c r="A53" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E52" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I52" s="14" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="60" x14ac:dyDescent="0.2">
-      <c r="A53" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D53" s="2" t="s">
+      <c r="E53" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="F53" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E53" s="17" t="s">
+      <c r="G53" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I53" s="14" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="F53" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="I53" s="14" t="s">
+      <c r="F54" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I54" s="15" t="s">
         <v>206</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="45" x14ac:dyDescent="0.2">
-      <c r="A54" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I54" s="15" t="s">
-        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>